<commit_message>
Working with Raport Table
</commit_message>
<xml_diff>
--- a/public/DataSiswa/Data Siswa.xlsx
+++ b/public/DataSiswa/Data Siswa.xlsx
@@ -1,27 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imbecile\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B772F6-B6CA-46C6-A23A-63C8276CC5E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
-  <si>
-    <t>andrew</t>
-  </si>
-  <si>
-    <t>Jakarta, 1 oktober 2000</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>002322567253</t>
   </si>
@@ -35,52 +42,149 @@
     <t>Bapak</t>
   </si>
   <si>
-    <t>2021-01-22T11:43:51.000000Z</t>
+    <t>32-123-324-56</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>IPS 3</t>
+  </si>
+  <si>
+    <t>IPS 1</t>
+  </si>
+  <si>
+    <t>32-87-83635</t>
+  </si>
+  <si>
+    <t>Padre</t>
+  </si>
+  <si>
+    <t>Nama Lengkap</t>
+  </si>
+  <si>
+    <t>TTL</t>
+  </si>
+  <si>
+    <t>NIS</t>
+  </si>
+  <si>
+    <t>NISN</t>
+  </si>
+  <si>
+    <t>Kelas</t>
+  </si>
+  <si>
+    <t>No Peserta</t>
+  </si>
+  <si>
+    <t>Billie Eilish</t>
+  </si>
+  <si>
+    <t>SF, 2 Februari 2020</t>
+  </si>
+  <si>
+    <t>James Morison</t>
+  </si>
+  <si>
+    <t>LA, 3 Maret 2020</t>
+  </si>
+  <si>
+    <t>Lil Pump</t>
+  </si>
+  <si>
+    <t>NY, 4 April 2020</t>
+  </si>
+  <si>
+    <t>Wali Murid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -370,62 +474,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1">
+    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3">
+        <v>15.766400000000001</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>15.7667</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3">
+        <v>15.879200000000001</v>
+      </c>
+      <c r="D3" s="4">
+        <v>8656890</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3">
+        <v>20.896699999999999</v>
+      </c>
+      <c r="D4" s="4">
+        <v>9274862387</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>